<commit_message>
fixed env file stuff
</commit_message>
<xml_diff>
--- a/examples/table_annotation/table_ANALYZED.xlsx
+++ b/examples/table_annotation/table_ANALYZED.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,15 +471,30 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Vertebrata_aln_property_entropy_z_score</t>
+          <t>Metazoa_aln_asym_sum_of_pairs_z_score</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>Metazoa_aln_slice_view</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Metazoa_cons_string</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Vertebrata_aln_asym_sum_of_pairs_z_score</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>Vertebrata_aln_slice_view</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Vertebrata_cons_string</t>
         </is>
@@ -514,6 +529,9 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -544,6 +562,9 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -570,17 +591,32 @@
           <t>conservation_analysis/2-9606_0_002f40/2-9606_0_002f40.json</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
+      <c r="G4">
+        <f>HYPERLINK("/Users/jackson/Dropbox (MIT)/work/07-SLiM_bioinformatics/05-conservation_pipeline/examples/table_annotation/conservation_analysis/2-9606_0_002f40/2-9606_0002f40-aln_asym_sum_of_pairs_og_level_score_screen.png")</f>
+        <v/>
+      </c>
       <c r="H4" t="n">
-        <v>-0.9222526690491762</v>
+        <v>-0.2623404708668192</v>
       </c>
       <c r="I4">
+        <f>HYPERLINK("conservation_analysis/2-9606_0_002f40/2-9606_0002f40-Metazoa_aln_slice.html")</f>
+        <v/>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>__SP_P_____</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>-0.2623404708668192</v>
+      </c>
+      <c r="L4">
         <f>HYPERLINK("conservation_analysis/2-9606_0_002f40/2-9606_0002f40-Vertebrata_aln_slice.html")</f>
         <v/>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>___P_______</t>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>__SP_P_____</t>
         </is>
       </c>
     </row>
@@ -609,15 +645,30 @@
           <t>conservation_analysis/3-9606_0_002f40/3-9606_0_002f40.json</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
+      <c r="G5">
+        <f>HYPERLINK("/Users/jackson/Dropbox (MIT)/work/07-SLiM_bioinformatics/05-conservation_pipeline/examples/table_annotation/conservation_analysis/3-9606_0_002f40/3-9606_0002f40-aln_asym_sum_of_pairs_og_level_score_screen.png")</f>
+        <v/>
+      </c>
       <c r="H5" t="n">
-        <v>-1.112491301468793</v>
+        <v>-1.164739051311995</v>
       </c>
       <c r="I5">
+        <f>HYPERLINK("conservation_analysis/3-9606_0_002f40/3-9606_0002f40-Metazoa_aln_slice.html")</f>
+        <v/>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>_______EE___</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>-1.164739051311995</v>
+      </c>
+      <c r="L5">
         <f>HYPERLINK("conservation_analysis/3-9606_0_002f40/3-9606_0002f40-Vertebrata_aln_slice.html")</f>
         <v/>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>_______EE___</t>
         </is>
@@ -656,6 +707,9 @@
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -690,6 +744,9 @@
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -724,6 +781,9 @@
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>